<commit_message>
ready for part 2
created 2 new variables and filled in numbers and answers
</commit_message>
<xml_diff>
--- a/starter-analysis-exercise/data/raw-data/exampledata 2.xlsx
+++ b/starter-analysis-exercise/data/raw-data/exampledata 2.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10114"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05288DF2-FCCB-C843-87F5-0F629B8BB93F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C2B9977-5D57-4644-873B-5DDC8A121C32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14480" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="23">
   <si>
     <t>Height</t>
   </si>
@@ -83,10 +83,13 @@
     <t>idetified smoking or not (yes/no)</t>
   </si>
   <si>
-    <t>Y/N</t>
-  </si>
-  <si>
-    <t>age in numver</t>
+    <t>age in number</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>Y/N/NA</t>
   </si>
 </sst>
 </file>
@@ -415,8 +418,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -449,6 +452,12 @@
       <c r="C2" t="s">
         <v>3</v>
       </c>
+      <c r="D2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2">
+        <v>76</v>
+      </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3">
@@ -460,6 +469,12 @@
       <c r="C3" t="s">
         <v>11</v>
       </c>
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3">
+        <v>11</v>
+      </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
@@ -471,6 +486,12 @@
       <c r="C4" t="s">
         <v>4</v>
       </c>
+      <c r="D4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4">
+        <v>44</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5">
@@ -482,6 +503,12 @@
       <c r="C5" t="s">
         <v>4</v>
       </c>
+      <c r="D5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5">
+        <v>48</v>
+      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6">
@@ -493,6 +520,12 @@
       <c r="C6" t="s">
         <v>5</v>
       </c>
+      <c r="D6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6">
+        <v>79</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7">
@@ -504,6 +537,12 @@
       <c r="C7" t="s">
         <v>4</v>
       </c>
+      <c r="D7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7">
+        <v>45</v>
+      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8">
@@ -515,6 +554,12 @@
       <c r="C8" t="s">
         <v>11</v>
       </c>
+      <c r="D8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8">
+        <v>30</v>
+      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9">
@@ -526,6 +571,12 @@
       <c r="C9" t="s">
         <v>3</v>
       </c>
+      <c r="D9" t="s">
+        <v>12</v>
+      </c>
+      <c r="E9">
+        <v>38</v>
+      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10">
@@ -537,6 +588,12 @@
       <c r="C10" t="s">
         <v>12</v>
       </c>
+      <c r="D10" t="s">
+        <v>12</v>
+      </c>
+      <c r="E10">
+        <v>27</v>
+      </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11">
@@ -548,6 +605,12 @@
       <c r="C11" t="s">
         <v>3</v>
       </c>
+      <c r="D11" t="s">
+        <v>21</v>
+      </c>
+      <c r="E11">
+        <v>19</v>
+      </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12">
@@ -556,6 +619,12 @@
       <c r="C12" t="s">
         <v>4</v>
       </c>
+      <c r="D12" t="s">
+        <v>12</v>
+      </c>
+      <c r="E12">
+        <v>51</v>
+      </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13">
@@ -567,6 +636,12 @@
       <c r="C13" t="s">
         <v>4</v>
       </c>
+      <c r="D13" t="s">
+        <v>5</v>
+      </c>
+      <c r="E13">
+        <v>20</v>
+      </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14">
@@ -578,6 +653,12 @@
       <c r="C14" t="s">
         <v>3</v>
       </c>
+      <c r="D14" t="s">
+        <v>12</v>
+      </c>
+      <c r="E14">
+        <v>35</v>
+      </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15">
@@ -588,6 +669,12 @@
       </c>
       <c r="C15" t="s">
         <v>3</v>
+      </c>
+      <c r="D15" t="s">
+        <v>21</v>
+      </c>
+      <c r="E15">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -599,8 +686,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4A2C8F0-62B4-4D60-B490-D490A3E0B40F}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -662,7 +749,7 @@
         <v>19</v>
       </c>
       <c r="C5" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -670,7 +757,7 @@
         <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C6" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
Prepared data for next step.
Added processed data as processed and processed2
</commit_message>
<xml_diff>
--- a/starter-analysis-exercise/data/raw-data/exampledata 2.xlsx
+++ b/starter-analysis-exercise/data/raw-data/exampledata 2.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C2B9977-5D57-4644-873B-5DDC8A121C32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71E4F62D-9159-4BD4-A087-878DB8F8D1F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-19320" yWindow="-120" windowWidth="19440" windowHeight="14880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -418,13 +418,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -442,7 +442,7 @@
       </c>
       <c r="G1" s="1"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A2">
         <v>180</v>
       </c>
@@ -459,7 +459,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A3">
         <v>175</v>
       </c>
@@ -476,7 +476,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -493,7 +493,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A5">
         <v>178</v>
       </c>
@@ -510,7 +510,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A6">
         <v>192</v>
       </c>
@@ -527,7 +527,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A7">
         <v>6</v>
       </c>
@@ -544,7 +544,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A8">
         <v>156</v>
       </c>
@@ -561,7 +561,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A9">
         <v>166</v>
       </c>
@@ -578,7 +578,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A10">
         <v>155</v>
       </c>
@@ -595,7 +595,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A11">
         <v>145</v>
       </c>
@@ -612,7 +612,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A12">
         <v>165</v>
       </c>
@@ -626,7 +626,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A13">
         <v>133</v>
       </c>
@@ -643,7 +643,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A14">
         <v>166</v>
       </c>
@@ -660,7 +660,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A15">
         <v>154</v>
       </c>
@@ -686,18 +686,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4A2C8F0-62B4-4D60-B490-D490A3E0B40F}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.33203125" customWidth="1"/>
-    <col min="3" max="3" width="21.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.3125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.3125" customWidth="1"/>
+    <col min="3" max="3" width="21.83984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -708,7 +708,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -719,7 +719,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -730,7 +730,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -741,7 +741,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -752,7 +752,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>18</v>
       </c>

</xml_diff>